<commit_message>
updated lots of stuff
</commit_message>
<xml_diff>
--- a/Nuclear_Fuel_Performance/NE591_Spring2020/grading.xlsx
+++ b/Nuclear_Fuel_Performance/NE591_Spring2020/grading.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/beelbw/projects/TEACHING/Nuclear_Fuel_Performance/NE591_Spring2020/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C6352847-F6C7-C147-8B26-CC845AAFB928}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB453DC5-3C6E-FC40-95B5-0E75930E25C6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11980" yWindow="5960" windowWidth="27640" windowHeight="16940" xr2:uid="{114B66FC-D05D-1747-9E35-A6C9832FE69D}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="19">
   <si>
     <t>Spring 2020</t>
   </si>
@@ -70,6 +70,18 @@
   </si>
   <si>
     <t>Letter</t>
+  </si>
+  <si>
+    <t>MOOSE Training</t>
+  </si>
+  <si>
+    <t>Presented project</t>
+  </si>
+  <si>
+    <t>possible</t>
+  </si>
+  <si>
+    <t>current</t>
   </si>
 </sst>
 </file>
@@ -421,20 +433,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78032B97-D432-2040-AA85-829DA4457FB6}">
-  <dimension ref="B2:P9"/>
+  <dimension ref="B2:S13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P6" sqref="P6"/>
+      <selection activeCell="S12" sqref="S12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="10" max="10" width="13.6640625" customWidth="1"/>
+    <col min="12" max="12" width="15.5" customWidth="1"/>
+    <col min="17" max="17" width="16.83203125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="2" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>0</v>
       </c>
@@ -463,22 +480,31 @@
         <v>9</v>
       </c>
       <c r="L5" t="s">
+        <v>16</v>
+      </c>
+      <c r="M5" t="s">
+        <v>9</v>
+      </c>
+      <c r="N5" t="s">
         <v>10</v>
       </c>
-      <c r="M5" t="s">
+      <c r="O5" t="s">
         <v>6</v>
       </c>
-      <c r="N5" t="s">
+      <c r="P5" t="s">
         <v>12</v>
       </c>
-      <c r="O5" t="s">
+      <c r="Q5" t="s">
+        <v>15</v>
+      </c>
+      <c r="R5" t="s">
         <v>13</v>
       </c>
-      <c r="P5" t="s">
+      <c r="S5" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:19" x14ac:dyDescent="0.2">
       <c r="E6">
         <v>0.2</v>
       </c>
@@ -489,17 +515,20 @@
         <v>0.2</v>
       </c>
       <c r="K6">
-        <v>0.15</v>
+        <v>0.1</v>
       </c>
       <c r="M6">
-        <v>0.25</v>
-      </c>
-      <c r="N6">
-        <f>SUM(E6:M6)</f>
+        <v>0.1</v>
+      </c>
+      <c r="O6">
+        <v>0.2</v>
+      </c>
+      <c r="P6">
+        <f>SUM(E6:O6)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
         <v>2</v>
       </c>
@@ -510,12 +539,12 @@
         <f>D7*$E$6</f>
         <v>12.200000000000001</v>
       </c>
-      <c r="O7">
-        <f>SUM(E7,G7,I7,K7,M7)</f>
+      <c r="R7">
+        <f>SUM(Q7,E7,G7,I7,K7,O7)</f>
         <v>12.200000000000001</v>
       </c>
     </row>
-    <row r="8" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
         <v>3</v>
       </c>
@@ -523,15 +552,15 @@
         <v>97</v>
       </c>
       <c r="E8">
-        <f t="shared" ref="E8:E9" si="0">D8*$E$6</f>
+        <f t="shared" ref="E8:E11" si="0">D8*$E$6</f>
         <v>19.400000000000002</v>
       </c>
-      <c r="O8">
-        <f>SUM(E8,G8,I8,K8,M8)</f>
+      <c r="R8">
+        <f t="shared" ref="R8:R9" si="1">SUM(Q8,E8,G8,I8,K8,O8)</f>
         <v>19.400000000000002</v>
       </c>
     </row>
-    <row r="9" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
         <v>4</v>
       </c>
@@ -542,9 +571,46 @@
         <f t="shared" si="0"/>
         <v>17.8</v>
       </c>
-      <c r="O9">
-        <f>SUM(E9,G9,I9,K9,M9)</f>
+      <c r="R9">
+        <f t="shared" si="1"/>
         <v>17.8</v>
+      </c>
+    </row>
+    <row r="10" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="R10" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="C11" t="s">
+        <v>17</v>
+      </c>
+      <c r="D11">
+        <v>100</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="P11">
+        <f>SUM(E11:O11)</f>
+        <v>20</v>
+      </c>
+      <c r="R11">
+        <f>R7/$P$11</f>
+        <v>0.6100000000000001</v>
+      </c>
+    </row>
+    <row r="12" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="R12">
+        <f t="shared" ref="R12:R13" si="2">R8/$P$11</f>
+        <v>0.97000000000000008</v>
+      </c>
+    </row>
+    <row r="13" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="R13">
+        <f t="shared" si="2"/>
+        <v>0.89</v>
       </c>
     </row>
   </sheetData>

</xml_diff>